<commit_message>
fix a bug of order of sort
</commit_message>
<xml_diff>
--- a/result/ans.xlsx
+++ b/result/ans.xlsx
@@ -16,51 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>threshold</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">passjoin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">过滤后结果数</t>
-    </r>
+    <t>passjoin过滤后结果数</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">passjoin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">最终结果数</t>
-    </r>
+    <t>string edit distance过滤后结果数</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Tree edit distance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF3C3C3C"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">最终结果数</t>
-    </r>
+    <t>最终结果数</t>
   </si>
   <si>
     <r>
@@ -105,12 +72,10 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">过滤后结果数</t>
     </r>
-  </si>
-  <si>
-    <t>最终结果数</t>
   </si>
   <si>
     <r>
@@ -121,6 +86,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">所用时间</t>
     </r>
@@ -134,6 +100,7 @@
         <sz val="10"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">所用时间</t>
     </r>
@@ -149,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -180,20 +147,9 @@
     <font>
       <sz val="10"/>
       <color rgb="FF3C3C3C"/>
-      <name val="Ubuntu"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF3C3C3C"/>
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Droid Sans Fallback"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -238,12 +194,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -251,11 +203,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -338,15 +286,15 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.280612244898"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.6683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.8316326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.484693877551"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7040816326531"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3367346938776"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.280612244898"/>
@@ -357,13 +305,13 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
@@ -372,7 +320,7 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -875,7 +823,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -895,25 +843,25 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -922,7 +870,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1096209</v>
+        <v>1081</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1047</v>
@@ -931,7 +879,7 @@
         <v>1047</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>0</v>
@@ -941,7 +889,7 @@
       </c>
       <c r="H2" s="0" t="n">
         <f aca="false">E2+F2+G2</f>
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -949,7 +897,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1096209</v>
+        <v>1281</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1089</v>
@@ -958,7 +906,7 @@
         <v>1089</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>0</v>
@@ -968,7 +916,7 @@
       </c>
       <c r="H3" s="0" t="n">
         <f aca="false">E3+F3+G3</f>
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -976,7 +924,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1096209</v>
+        <v>2003</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1331</v>
@@ -985,7 +933,7 @@
         <v>1331</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>0</v>
@@ -995,7 +943,7 @@
       </c>
       <c r="H4" s="0" t="n">
         <f aca="false">E4+F4+G4</f>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,7 +951,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1096209</v>
+        <v>2471</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1465</v>
@@ -1012,7 +960,7 @@
         <v>1465</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>0</v>
@@ -1022,7 +970,7 @@
       </c>
       <c r="H5" s="0" t="n">
         <f aca="false">E5+F5+G5</f>
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,7 +978,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1096209</v>
+        <v>2893</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1511</v>
@@ -1039,7 +987,7 @@
         <v>1511</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>0</v>
@@ -1049,7 +997,7 @@
       </c>
       <c r="H6" s="0" t="n">
         <f aca="false">E6+F6+G6</f>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1057,7 +1005,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1096209</v>
+        <v>3731</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1555</v>
@@ -1066,7 +1014,7 @@
         <v>1555</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>0</v>
@@ -1076,7 +1024,7 @@
       </c>
       <c r="H7" s="0" t="n">
         <f aca="false">E7+F7+G7</f>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,7 +1032,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>1096209</v>
+        <v>4651</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1595</v>
@@ -1093,7 +1041,7 @@
         <v>1595</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>0</v>
@@ -1103,7 +1051,7 @@
       </c>
       <c r="H8" s="0" t="n">
         <f aca="false">E8+F8+G8</f>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1111,7 +1059,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1096209</v>
+        <v>6511</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1661</v>
@@ -1120,7 +1068,7 @@
         <v>1661</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>1</v>
@@ -1130,7 +1078,7 @@
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">E9+F9+G9</f>
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1138,7 +1086,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1096209</v>
+        <v>9243</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1775</v>
@@ -1147,7 +1095,7 @@
         <v>1775</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>1</v>
@@ -1157,7 +1105,7 @@
       </c>
       <c r="H10" s="0" t="n">
         <f aca="false">E10+F10+G10</f>
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1165,7 +1113,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1096209</v>
+        <v>12359</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1987</v>
@@ -1174,7 +1122,7 @@
         <v>1987</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>1</v>
@@ -1184,7 +1132,7 @@
       </c>
       <c r="H11" s="0" t="n">
         <f aca="false">E11+F11+G11</f>
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1192,7 +1140,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>1096209</v>
+        <v>17607</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>2109</v>
@@ -1201,7 +1149,7 @@
         <v>2109</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>2</v>
@@ -1211,7 +1159,7 @@
       </c>
       <c r="H12" s="0" t="n">
         <f aca="false">E12+F12+G12</f>
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1219,7 +1167,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>1096209</v>
+        <v>24277</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>2223</v>
@@ -1228,7 +1176,7 @@
         <v>2223</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>2</v>
@@ -1238,7 +1186,7 @@
       </c>
       <c r="H13" s="0" t="n">
         <f aca="false">E13+F13+G13</f>
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,7 +1194,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>1096209</v>
+        <v>35283</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>2375</v>
@@ -1255,7 +1203,7 @@
         <v>2375</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>3</v>
@@ -1265,7 +1213,7 @@
       </c>
       <c r="H14" s="0" t="n">
         <f aca="false">E14+F14+G14</f>
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,7 +1221,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>1096209</v>
+        <v>50641</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>2481</v>
@@ -1282,7 +1230,7 @@
         <v>2477</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>3</v>
@@ -1292,7 +1240,7 @@
       </c>
       <c r="H15" s="0" t="n">
         <f aca="false">E15+F15+G15</f>
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,7 +1248,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>1096209</v>
+        <v>69357</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>2837</v>
@@ -1309,7 +1257,7 @@
         <v>2821</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>4</v>
@@ -1319,7 +1267,7 @@
       </c>
       <c r="H16" s="0" t="n">
         <f aca="false">E16+F16+G16</f>
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,7 +1275,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>1096209</v>
+        <v>88315</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>3179</v>
@@ -1336,7 +1284,7 @@
         <v>3157</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>4</v>
@@ -1346,7 +1294,7 @@
       </c>
       <c r="H17" s="0" t="n">
         <f aca="false">E17+F17+G17</f>
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1354,7 +1302,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>1096209</v>
+        <v>115533</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>3373</v>
@@ -1363,7 +1311,7 @@
         <v>3345</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>5</v>
@@ -1373,7 +1321,7 @@
       </c>
       <c r="H18" s="0" t="n">
         <f aca="false">E18+F18+G18</f>
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1381,7 +1329,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>1096209</v>
+        <v>143209</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>3857</v>
@@ -1390,7 +1338,7 @@
         <v>3813</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>4</v>
@@ -1400,7 +1348,7 @@
       </c>
       <c r="H19" s="0" t="n">
         <f aca="false">E19+F19+G19</f>
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1408,7 +1356,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>1096209</v>
+        <v>173935</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>4195</v>
@@ -1417,7 +1365,7 @@
         <v>4107</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>5</v>
@@ -1427,7 +1375,7 @@
       </c>
       <c r="H20" s="0" t="n">
         <f aca="false">E20+F20+G20</f>
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1435,7 +1383,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>1096209</v>
+        <v>208665</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>4679</v>
@@ -1444,7 +1392,7 @@
         <v>4527</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>6</v>
@@ -1454,7 +1402,7 @@
       </c>
       <c r="H21" s="0" t="n">
         <f aca="false">E21+F21+G21</f>
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add some code to delete dynamic arrays. Now I need to find some bigger data
</commit_message>
<xml_diff>
--- a/result/ans.xlsx
+++ b/result/ans.xlsx
@@ -286,8 +286,8 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -341,11 +341,11 @@
         <v>0</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G2" s="0" t="n">
         <f aca="false">E2+F2</f>
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -365,11 +365,11 @@
         <v>0</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G3" s="0" t="n">
         <f aca="false">E3+F3</f>
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -389,11 +389,11 @@
         <v>0</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="n">
         <f aca="false">E4+F4</f>
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,11 +413,11 @@
         <v>0</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G5" s="0" t="n">
         <f aca="false">E5+F5</f>
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -437,11 +437,11 @@
         <v>0</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">E6+F6</f>
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -461,11 +461,11 @@
         <v>0</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">E7+F7</f>
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -485,11 +485,11 @@
         <v>0</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">E8+F8</f>
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -509,11 +509,11 @@
         <v>0</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">E9+F9</f>
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -530,14 +530,14 @@
         <v>1775</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G10" s="0" t="n">
         <f aca="false">E10+F10</f>
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -557,11 +557,11 @@
         <v>1</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">E11+F11</f>
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -581,11 +581,11 @@
         <v>1</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">E12+F12</f>
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -602,14 +602,14 @@
         <v>2223</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">E13+F13</f>
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -629,11 +629,11 @@
         <v>2</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">E14+F14</f>
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,11 +653,11 @@
         <v>2</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G15" s="0" t="n">
         <f aca="false">E15+F15</f>
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -674,14 +674,14 @@
         <v>2821</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">E16+F16</f>
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -701,11 +701,11 @@
         <v>3</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G17" s="0" t="n">
         <f aca="false">E17+F17</f>
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -722,14 +722,14 @@
         <v>3345</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G18" s="0" t="n">
         <f aca="false">E18+F18</f>
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -746,14 +746,14 @@
         <v>3813</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="G19" s="0" t="n">
         <f aca="false">E19+F19</f>
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -770,14 +770,14 @@
         <v>4107</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="G20" s="0" t="n">
         <f aca="false">E20+F20</f>
-        <v>64</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,14 +794,14 @@
         <v>4527</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="G21" s="0" t="n">
         <f aca="false">E21+F21</f>
-        <v>70</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -823,7 +823,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -885,11 +885,11 @@
         <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H2" s="0" t="n">
         <f aca="false">E2+F2+G2</f>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -912,11 +912,11 @@
         <v>0</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H3" s="0" t="n">
         <f aca="false">E3+F3+G3</f>
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -939,11 +939,11 @@
         <v>0</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="H4" s="0" t="n">
         <f aca="false">E4+F4+G4</f>
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -966,11 +966,11 @@
         <v>0</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="H5" s="0" t="n">
         <f aca="false">E5+F5+G5</f>
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -993,11 +993,11 @@
         <v>0</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="H6" s="0" t="n">
         <f aca="false">E6+F6+G6</f>
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1020,11 +1020,11 @@
         <v>0</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="H7" s="0" t="n">
         <f aca="false">E7+F7+G7</f>
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1047,11 +1047,11 @@
         <v>0</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="H8" s="0" t="n">
         <f aca="false">E8+F8+G8</f>
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1071,14 +1071,14 @@
         <v>0</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">E9+F9+G9</f>
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,14 +1098,14 @@
         <v>0</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="H10" s="0" t="n">
         <f aca="false">E10+F10+G10</f>
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1125,14 +1125,14 @@
         <v>0</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="H11" s="0" t="n">
         <f aca="false">E11+F11+G11</f>
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,14 +1152,14 @@
         <v>0</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H12" s="0" t="n">
         <f aca="false">E12+F12+G12</f>
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1179,14 +1179,14 @@
         <v>0</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="H13" s="0" t="n">
         <f aca="false">E13+F13+G13</f>
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,14 +1206,14 @@
         <v>0</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="H14" s="0" t="n">
         <f aca="false">E14+F14+G14</f>
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1233,14 +1233,14 @@
         <v>0</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="H15" s="0" t="n">
         <f aca="false">E15+F15+G15</f>
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1260,14 +1260,14 @@
         <v>0</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="H16" s="0" t="n">
         <f aca="false">E16+F16+G16</f>
-        <v>51</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1287,14 +1287,14 @@
         <v>0</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="H17" s="0" t="n">
         <f aca="false">E17+F17+G17</f>
-        <v>54</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,14 +1314,14 @@
         <v>0</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="H18" s="0" t="n">
         <f aca="false">E18+F18+G18</f>
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1341,14 +1341,14 @@
         <v>0</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="H19" s="0" t="n">
         <f aca="false">E19+F19+G19</f>
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1368,14 +1368,14 @@
         <v>0</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="H20" s="0" t="n">
         <f aca="false">E20+F20+G20</f>
-        <v>59</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1395,14 +1395,14 @@
         <v>0</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="H21" s="0" t="n">
         <f aca="false">E21+F21+G21</f>
-        <v>68</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>